<commit_message>
add dictionary excel and testing excels
</commit_message>
<xml_diff>
--- a/Examples/Dictionary/Calc/Exp119_Excel_sensitivity.xlsx
+++ b/Examples/Dictionary/Calc/Exp119_Excel_sensitivity.xlsx
@@ -155,6 +155,174 @@
     </pic>
     <clientData/>
   </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6096000" cy="4572000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6096000" cy="4572000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6096000" cy="4572000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6096000" cy="4572000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="5" name="Image 5" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6096000" cy="4572000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="6" name="Image 6" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6096000" cy="4572000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="7" name="Image 7" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -175,6 +343,174 @@
       </nvPicPr>
       <blipFill>
         <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6096000" cy="4572000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="2" name="Image 2" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6096000" cy="4572000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="3" name="Image 3" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6096000" cy="4572000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="4" name="Image 4" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6096000" cy="4572000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="5" name="Image 5" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6096000" cy="4572000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="6" name="Image 6" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+        <a:ln>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>0</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="6096000" cy="4572000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="7" name="Image 7" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>

</xml_diff>